<commit_message>
fixing formatting in spreadsheet
</commit_message>
<xml_diff>
--- a/fpga_verification.xlsx
+++ b/fpga_verification.xlsx
@@ -518,7 +518,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -546,7 +546,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -576,8 +576,8 @@
   </sheetPr>
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>